<commit_message>
add technology & manage demandsassess
</commit_message>
<xml_diff>
--- a/d_up_loads/细则自评.xlsx
+++ b/d_up_loads/细则自评.xlsx
@@ -7,12 +7,13 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="工作表 1" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="538">
   <si>
     <t>等级</t>
   </si>
@@ -3450,6 +3451,54 @@
   </si>
   <si>
     <t>应随着信息系统的变更定期对原有的应急预案重新评估，修订完善</t>
+  </si>
+  <si>
+    <t>business_assess</t>
+  </si>
+  <si>
+    <t>业务信息安全保护等级自评</t>
+  </si>
+  <si>
+    <t>system_assess</t>
+  </si>
+  <si>
+    <t>系统服务安全保护等级自评</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>一般损害</t>
+  </si>
+  <si>
+    <t>serious</t>
+  </si>
+  <si>
+    <t>严重损害</t>
+  </si>
+  <si>
+    <t>sspecial</t>
+  </si>
+  <si>
+    <t>特别严重损害</t>
+  </si>
+  <si>
+    <t>citizen</t>
+  </si>
+  <si>
+    <t>公民、法人和其他组织的合法权益</t>
+  </si>
+  <si>
+    <t>social</t>
+  </si>
+  <si>
+    <t>社会秩序、公共利益</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>国家安全</t>
   </si>
 </sst>
 </file>
@@ -3492,7 +3541,7 @@
       <name val="黑体"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3511,8 +3560,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -3550,13 +3611,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -3617,11 +3783,44 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3643,6 +3842,10 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -10896,7 +11099,9 @@
       <c r="B14" t="s" s="15">
         <v>258</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" t="s" s="15">
+        <v>265</v>
+      </c>
       <c r="D14" t="s" s="14">
         <v>267</v>
       </c>
@@ -10921,7 +11126,7 @@
       <c r="A16" s="7">
         <v>1</v>
       </c>
-      <c r="B16" t="s" s="21">
+      <c r="B16" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C16" t="s" s="15">
@@ -10936,7 +11141,7 @@
       <c r="A17" s="7">
         <v>1</v>
       </c>
-      <c r="B17" t="s" s="21">
+      <c r="B17" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C17" t="s" s="15">
@@ -10951,7 +11156,7 @@
       <c r="A18" s="7">
         <v>1</v>
       </c>
-      <c r="B18" t="s" s="21">
+      <c r="B18" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C18" t="s" s="15">
@@ -10966,7 +11171,7 @@
       <c r="A19" s="7">
         <v>1</v>
       </c>
-      <c r="B19" t="s" s="21">
+      <c r="B19" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C19" t="s" s="15">
@@ -10981,7 +11186,7 @@
       <c r="A20" s="7">
         <v>1</v>
       </c>
-      <c r="B20" t="s" s="21">
+      <c r="B20" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C20" t="s" s="15">
@@ -10996,7 +11201,7 @@
       <c r="A21" s="7">
         <v>1</v>
       </c>
-      <c r="B21" t="s" s="21">
+      <c r="B21" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C21" t="s" s="15">
@@ -11011,7 +11216,7 @@
       <c r="A22" s="7">
         <v>1</v>
       </c>
-      <c r="B22" t="s" s="21">
+      <c r="B22" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C22" t="s" s="13">
@@ -11026,7 +11231,7 @@
       <c r="A23" s="7">
         <v>1</v>
       </c>
-      <c r="B23" t="s" s="21">
+      <c r="B23" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C23" t="s" s="15">
@@ -11041,7 +11246,7 @@
       <c r="A24" s="7">
         <v>1</v>
       </c>
-      <c r="B24" t="s" s="21">
+      <c r="B24" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C24" t="s" s="15">
@@ -11056,7 +11261,7 @@
       <c r="A25" s="7">
         <v>1</v>
       </c>
-      <c r="B25" t="s" s="21">
+      <c r="B25" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C25" t="s" s="15">
@@ -11071,7 +11276,7 @@
       <c r="A26" s="7">
         <v>1</v>
       </c>
-      <c r="B26" t="s" s="21">
+      <c r="B26" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C26" t="s" s="15">
@@ -11086,7 +11291,7 @@
       <c r="A27" s="7">
         <v>1</v>
       </c>
-      <c r="B27" t="s" s="21">
+      <c r="B27" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C27" t="s" s="15">
@@ -11101,7 +11306,7 @@
       <c r="A28" s="7">
         <v>1</v>
       </c>
-      <c r="B28" t="s" s="21">
+      <c r="B28" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C28" t="s" s="13">
@@ -11116,7 +11321,7 @@
       <c r="A29" s="7">
         <v>1</v>
       </c>
-      <c r="B29" t="s" s="21">
+      <c r="B29" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C29" t="s" s="15">
@@ -11131,7 +11336,7 @@
       <c r="A30" s="7">
         <v>1</v>
       </c>
-      <c r="B30" t="s" s="21">
+      <c r="B30" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C30" t="s" s="15">
@@ -11146,7 +11351,7 @@
       <c r="A31" s="7">
         <v>1</v>
       </c>
-      <c r="B31" t="s" s="21">
+      <c r="B31" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C31" t="s" s="15">
@@ -11161,7 +11366,7 @@
       <c r="A32" s="7">
         <v>1</v>
       </c>
-      <c r="B32" t="s" s="21">
+      <c r="B32" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C32" t="s" s="15">
@@ -11176,7 +11381,7 @@
       <c r="A33" s="7">
         <v>1</v>
       </c>
-      <c r="B33" t="s" s="21">
+      <c r="B33" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C33" t="s" s="15">
@@ -11191,7 +11396,7 @@
       <c r="A34" s="7">
         <v>1</v>
       </c>
-      <c r="B34" t="s" s="21">
+      <c r="B34" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C34" t="s" s="15">
@@ -11206,7 +11411,7 @@
       <c r="A35" s="7">
         <v>1</v>
       </c>
-      <c r="B35" t="s" s="21">
+      <c r="B35" t="s" s="20">
         <v>270</v>
       </c>
       <c r="C35" t="s" s="15">
@@ -17899,4 +18104,157 @@
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="21" customWidth="1"/>
+    <col min="2" max="2" width="18" style="21" customWidth="1"/>
+    <col min="3" max="3" width="25.8516" style="21" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="21" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="21" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.55" customHeight="1">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" ht="15.55" customHeight="1">
+      <c r="A2" s="23">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="24">
+        <v>522</v>
+      </c>
+      <c r="C2" t="s" s="25">
+        <v>523</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+    </row>
+    <row r="3" ht="15.35" customHeight="1">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="28">
+        <v>524</v>
+      </c>
+      <c r="C3" t="s" s="29">
+        <v>525</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+    </row>
+    <row r="4" ht="15.35" customHeight="1">
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+    </row>
+    <row r="5" ht="15.35" customHeight="1">
+      <c r="A5" s="27">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s" s="28">
+        <v>526</v>
+      </c>
+      <c r="C5" t="s" s="29">
+        <v>527</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" ht="15.35" customHeight="1">
+      <c r="A6" s="27">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s" s="28">
+        <v>528</v>
+      </c>
+      <c r="C6" t="s" s="29">
+        <v>529</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1">
+      <c r="A7" s="27">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s" s="28">
+        <v>530</v>
+      </c>
+      <c r="C7" t="s" s="29">
+        <v>531</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" ht="15.35" customHeight="1">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="27">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s" s="28">
+        <v>532</v>
+      </c>
+      <c r="C9" t="s" s="29">
+        <v>533</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="27">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s" s="28">
+        <v>534</v>
+      </c>
+      <c r="C10" t="s" s="29">
+        <v>535</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+    </row>
+    <row r="11" ht="15.35" customHeight="1">
+      <c r="A11" s="27">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s" s="28">
+        <v>536</v>
+      </c>
+      <c r="C11" t="s" s="29">
+        <v>537</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>